<commit_message>
update assertion on sorting
</commit_message>
<xml_diff>
--- a/Test Case_Sauce Demo.xlsx
+++ b/Test Case_Sauce Demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Katalon Studio\sauceDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Playwright\OrangeHRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D8BE01-BC39-461C-BB37-E976EF11CDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4E1E0E-ADD9-4607-A692-EF585A6D5236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,9 +586,6 @@
 7. Klik ikon Shopping Cart (keranjang). dibagian pojok kanan</t>
   </si>
   <si>
-    <t>Verifikasi pengurutan 'Price (low to high)' tidak kembali ke default (reset) saat halaman dimuat ulang</t>
-  </si>
-  <si>
     <t>S2</t>
   </si>
   <si>
@@ -722,6 +719,9 @@
   </si>
   <si>
     <t>HP_SCN_003_TC_CART_005</t>
+  </si>
+  <si>
+    <t>Verifikasi pengurutan 'Name (Z - A)' tidak kembali ke default (reset) saat halaman dimuat ulang</t>
   </si>
 </sst>
 </file>
@@ -1043,33 +1043,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1118,13 +1091,31 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1138,6 +1129,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1731,16 +1731,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="33" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1752,16 +1752,16 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="36">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="27">
         <v>46113</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1773,16 +1773,16 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1794,11 +1794,11 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -1819,9 +1819,9 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="11">
         <v>0</v>
       </c>
@@ -1923,121 +1923,121 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="31">
         <v>1</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12" t="s">
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
     </row>
     <row r="13" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
     </row>
     <row r="14" spans="1:15" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="8" t="s">
         <v>60</v>
       </c>
@@ -2075,102 +2075,102 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="A15" s="31">
         <v>3</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="12" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="18" t="s">
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="19"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="35"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="19"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="35"/>
     </row>
     <row r="18" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="20"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="36"/>
     </row>
     <row r="19" spans="1:15" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>4</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="8" t="s">
         <v>60</v>
       </c>
@@ -2211,7 +2211,7 @@
       <c r="A20" s="7">
         <v>5</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="8" t="s">
         <v>60</v>
       </c>
@@ -2252,7 +2252,7 @@
       <c r="A21" s="7">
         <v>6</v>
       </c>
-      <c r="B21" s="16"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="8" t="s">
         <v>60</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="A22" s="7">
         <v>7</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="8" t="s">
         <v>60</v>
       </c>
@@ -2334,7 +2334,7 @@
       <c r="A23" s="7">
         <v>8</v>
       </c>
-      <c r="B23" s="16"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="8" t="s">
         <v>60</v>
       </c>
@@ -2375,7 +2375,7 @@
       <c r="A24" s="7">
         <v>9</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="8" t="s">
         <v>60</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="A25" s="7">
         <v>10</v>
       </c>
-      <c r="B25" s="16"/>
+      <c r="B25" s="32"/>
       <c r="C25" s="8" t="s">
         <v>60</v>
       </c>
@@ -2457,7 +2457,7 @@
       <c r="A26" s="7">
         <v>11</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="8" t="s">
         <v>60</v>
       </c>
@@ -2498,7 +2498,7 @@
       <c r="A27" s="7">
         <v>12</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="8" t="s">
         <v>60</v>
       </c>
@@ -2536,102 +2536,102 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28" s="31">
         <v>13</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="12" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="G28" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="J28" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="K28" s="12" t="s">
+      <c r="K28" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="L28" s="12" t="s">
+      <c r="L28" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="18" t="s">
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="19"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="35"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="19"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="35"/>
     </row>
     <row r="31" spans="1:15" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="20"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="36"/>
     </row>
     <row r="32" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>14</v>
       </c>
-      <c r="B32" s="16"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="8" t="s">
         <v>51</v>
       </c>
@@ -2672,7 +2672,7 @@
       <c r="A33" s="7">
         <v>15</v>
       </c>
-      <c r="B33" s="16"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="8" t="s">
         <v>51</v>
       </c>
@@ -2714,7 +2714,7 @@
         <f>SUM(A33+1)</f>
         <v>16</v>
       </c>
-      <c r="B34" s="16"/>
+      <c r="B34" s="32"/>
       <c r="C34" s="8" t="s">
         <v>51</v>
       </c>
@@ -2756,7 +2756,7 @@
         <f t="shared" ref="A35:A36" si="0">SUM(A34+1)</f>
         <v>17</v>
       </c>
-      <c r="B35" s="16"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="8" t="s">
         <v>51</v>
       </c>
@@ -2798,7 +2798,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B36" s="17"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="8" t="s">
         <v>51</v>
       </c>
@@ -2837,13 +2837,33 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="B9:B36"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="H9:H13"/>
+    <mergeCell ref="I9:I13"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="O28:O31"/>
+    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="M15:M18"/>
+    <mergeCell ref="N15:N18"/>
+    <mergeCell ref="O15:O18"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="K28:K31"/>
+    <mergeCell ref="L28:L31"/>
+    <mergeCell ref="M28:M31"/>
+    <mergeCell ref="N28:N31"/>
     <mergeCell ref="N9:N13"/>
     <mergeCell ref="O9:O13"/>
     <mergeCell ref="A15:A18"/>
@@ -2860,33 +2880,13 @@
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="L9:L13"/>
     <mergeCell ref="M9:M13"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="K28:K31"/>
-    <mergeCell ref="L28:L31"/>
-    <mergeCell ref="M28:M31"/>
-    <mergeCell ref="N28:N31"/>
-    <mergeCell ref="O28:O31"/>
-    <mergeCell ref="L15:L18"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="N15:N18"/>
-    <mergeCell ref="O15:O18"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="H9:H13"/>
-    <mergeCell ref="I9:I13"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="D9:D13"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="B9:B36"/>
-    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="G19:I28 G32:I36">
@@ -2987,10 +2987,10 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3013,16 +3013,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="33" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -3034,16 +3034,16 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="36">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="27">
         <v>46113</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3055,16 +3055,16 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3076,11 +3076,11 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -3101,9 +3101,9 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="11">
         <v>0</v>
       </c>
@@ -3205,124 +3205,124 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="37">
+      <c r="A9" s="41">
         <v>1</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12" t="s">
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
     </row>
     <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>123</v>
@@ -3355,107 +3355,107 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="37">
+      <c r="A15" s="41">
         <v>3</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="E15" s="38" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="18" t="s">
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="19"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="35"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="19"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="35"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="20"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="36"/>
     </row>
     <row r="19" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>4</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>141</v>
@@ -3491,10 +3491,10 @@
       <c r="A20" s="7">
         <v>5</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>142</v>
@@ -3530,10 +3530,10 @@
       <c r="A21" s="7">
         <v>6</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>134</v>
@@ -3570,10 +3570,10 @@
         <f>SUM(A21+1)</f>
         <v>7</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>143</v>
@@ -3610,13 +3610,13 @@
         <f t="shared" ref="A23" si="0">SUM(A22+1)</f>
         <v>8</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>127</v>
@@ -3628,16 +3628,16 @@
         <v>102</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>103</v>
       </c>
       <c r="K23" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="L23" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
@@ -3648,14 +3648,14 @@
         <f>SUM(A23+1)</f>
         <v>9</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="34" t="s">
         <v>140</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>145</v>
@@ -3676,7 +3676,7 @@
         <v>103</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>147</v>
@@ -3692,10 +3692,10 @@
         <f>SUM(A24+1)</f>
         <v>10</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>144</v>
@@ -3716,7 +3716,7 @@
         <v>103</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>146</v>
@@ -3732,13 +3732,13 @@
         <f t="shared" ref="A26:A28" si="1">SUM(A25+1)</f>
         <v>11</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>127</v>
@@ -3747,19 +3747,19 @@
         <v>20</v>
       </c>
       <c r="H26" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="I26" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>103</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
@@ -3770,13 +3770,13 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>127</v>
@@ -3785,19 +3785,19 @@
         <v>21</v>
       </c>
       <c r="H27" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="I27" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>103</v>
       </c>
       <c r="K27" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="L27" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
@@ -3808,13 +3808,13 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
       <c r="D28" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>127</v>
@@ -3832,10 +3832,10 @@
         <v>103</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
@@ -3845,17 +3845,18 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="K15:K18"/>
+    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="M15:M18"/>
+    <mergeCell ref="L9:L13"/>
+    <mergeCell ref="M9:M13"/>
+    <mergeCell ref="N9:N13"/>
+    <mergeCell ref="O9:O13"/>
+    <mergeCell ref="N15:N18"/>
+    <mergeCell ref="O15:O18"/>
     <mergeCell ref="J9:J13"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="A9:A13"/>
@@ -3872,18 +3873,17 @@
     <mergeCell ref="D15:D18"/>
     <mergeCell ref="E15:E18"/>
     <mergeCell ref="F15:F18"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="L9:L13"/>
-    <mergeCell ref="M9:M13"/>
-    <mergeCell ref="N9:N13"/>
-    <mergeCell ref="O9:O13"/>
-    <mergeCell ref="N15:N18"/>
-    <mergeCell ref="O15:O18"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="J15:J18"/>
-    <mergeCell ref="K15:K18"/>
-    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="B24:B28"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="G19:I28">
@@ -3987,16 +3987,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="33" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -4008,16 +4008,16 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="36">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="27">
         <v>46113</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -4029,16 +4029,16 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -4050,11 +4050,11 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -4075,9 +4075,9 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="11">
         <v>0</v>
       </c>
@@ -4183,13 +4183,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>140</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>145</v>
@@ -4229,7 +4229,7 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>144</v>
@@ -4269,7 +4269,7 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
refactor: enhance CartPage functionality and update test cases
</commit_message>
<xml_diff>
--- a/Test Case_Sauce Demo.xlsx
+++ b/Test Case_Sauce Demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Playwright\OrangeHRM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Playwright\SauceDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0E0C3B-0D6E-418D-8F9D-67D9826CC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7951D5AC-0AC1-42DA-82F3-5230636E78C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -690,13 +690,6 @@
     <t>Sistem mengarahkan pengguna ke halaman "Checkout: Your Information" (halaman pengisian data diri).</t>
   </si>
   <si>
-    <t>1. Isi field Username dengan data valid
-2. Isi field Password dengan "invalid_password" 
-3. Klik tombol "Login"
-4. Klik ikon keranjang untuk masuk ke halaman Your Cart.
-5. Periksa keberadaan tombol "Checkout" atau pesan informasi.</t>
-  </si>
-  <si>
     <t>Tombol "Checkout" tidak merespon/tidak ada, atau muncul pesan informatif bahwa keranjang masih kosong.</t>
   </si>
   <si>
@@ -722,6 +715,12 @@
   </si>
   <si>
     <t>CP_SCN_001</t>
+  </si>
+  <si>
+    <t>1. Isi field Username dengan data valid
+2. Klik tombol "Login"
+3. Klik ikon keranjang untuk masuk ke halaman Your Cart.
+4. Periksa keberadaan tombol "Checkout" atau pesan informasi.</t>
   </si>
 </sst>
 </file>
@@ -1043,6 +1042,36 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1091,31 +1120,13 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1129,18 +1140,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1734,16 +1733,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="24" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1755,16 +1754,16 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="27">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="37">
         <v>46113</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1776,16 +1775,16 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1797,11 +1796,11 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -1822,9 +1821,9 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="11">
         <v>0</v>
       </c>
@@ -1926,121 +1925,121 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
+      <c r="A9" s="16">
         <v>1</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="L9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28" t="s">
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
     </row>
     <row r="13" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
     </row>
     <row r="14" spans="1:15" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="32"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="8" t="s">
         <v>59</v>
       </c>
@@ -2078,102 +2077,102 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31">
+      <c r="A15" s="16">
         <v>3</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="28" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="G15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="28" t="s">
+      <c r="K15" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="L15" s="28" t="s">
+      <c r="L15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="34" t="s">
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="35"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="20"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="35"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="20"/>
     </row>
     <row r="18" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="36"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="21"/>
     </row>
     <row r="19" spans="1:15" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>4</v>
       </c>
-      <c r="B19" s="32"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="8" t="s">
         <v>59</v>
       </c>
@@ -2214,7 +2213,7 @@
       <c r="A20" s="7">
         <v>5</v>
       </c>
-      <c r="B20" s="32"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="8" t="s">
         <v>59</v>
       </c>
@@ -2255,7 +2254,7 @@
       <c r="A21" s="7">
         <v>6</v>
       </c>
-      <c r="B21" s="32"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="8" t="s">
         <v>59</v>
       </c>
@@ -2296,7 +2295,7 @@
       <c r="A22" s="7">
         <v>7</v>
       </c>
-      <c r="B22" s="32"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="8" t="s">
         <v>59</v>
       </c>
@@ -2337,7 +2336,7 @@
       <c r="A23" s="7">
         <v>8</v>
       </c>
-      <c r="B23" s="32"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="8" t="s">
         <v>59</v>
       </c>
@@ -2378,7 +2377,7 @@
       <c r="A24" s="7">
         <v>9</v>
       </c>
-      <c r="B24" s="32"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="8" t="s">
         <v>59</v>
       </c>
@@ -2419,7 +2418,7 @@
       <c r="A25" s="7">
         <v>10</v>
       </c>
-      <c r="B25" s="32"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="8" t="s">
         <v>59</v>
       </c>
@@ -2460,7 +2459,7 @@
       <c r="A26" s="7">
         <v>11</v>
       </c>
-      <c r="B26" s="32"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="8" t="s">
         <v>59</v>
       </c>
@@ -2501,7 +2500,7 @@
       <c r="A27" s="7">
         <v>12</v>
       </c>
-      <c r="B27" s="32"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="8" t="s">
         <v>59</v>
       </c>
@@ -2539,102 +2538,102 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31">
+      <c r="A28" s="16">
         <v>13</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="28" t="s">
+      <c r="B28" s="17"/>
+      <c r="C28" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="28" t="s">
+      <c r="F28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="34" t="s">
+      <c r="G28" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="34" t="s">
+      <c r="H28" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="28" t="s">
+      <c r="J28" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="K28" s="28" t="s">
+      <c r="K28" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="L28" s="28" t="s">
+      <c r="L28" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="34" t="s">
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
-      <c r="O29" s="35"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="20"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="35"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="20"/>
     </row>
     <row r="31" spans="1:15" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="36"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="21"/>
     </row>
     <row r="32" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>14</v>
       </c>
-      <c r="B32" s="32"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="8" t="s">
         <v>51</v>
       </c>
@@ -2675,7 +2674,7 @@
       <c r="A33" s="7">
         <v>15</v>
       </c>
-      <c r="B33" s="32"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="8" t="s">
         <v>51</v>
       </c>
@@ -2717,7 +2716,7 @@
         <f>SUM(A33+1)</f>
         <v>16</v>
       </c>
-      <c r="B34" s="32"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="8" t="s">
         <v>51</v>
       </c>
@@ -2759,7 +2758,7 @@
         <f t="shared" ref="A35:A36" si="0">SUM(A34+1)</f>
         <v>17</v>
       </c>
-      <c r="B35" s="32"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="8" t="s">
         <v>51</v>
       </c>
@@ -2801,7 +2800,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B36" s="33"/>
+      <c r="B36" s="18"/>
       <c r="C36" s="8" t="s">
         <v>51</v>
       </c>
@@ -2840,33 +2839,13 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="D9:D13"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="B9:B36"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="H9:H13"/>
-    <mergeCell ref="I9:I13"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="O28:O31"/>
-    <mergeCell ref="L15:L18"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="N15:N18"/>
-    <mergeCell ref="O15:O18"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="K28:K31"/>
-    <mergeCell ref="L28:L31"/>
-    <mergeCell ref="M28:M31"/>
-    <mergeCell ref="N28:N31"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
     <mergeCell ref="N9:N13"/>
     <mergeCell ref="O9:O13"/>
     <mergeCell ref="A15:A18"/>
@@ -2883,13 +2862,33 @@
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="L9:L13"/>
     <mergeCell ref="M9:M13"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="K28:K31"/>
+    <mergeCell ref="L28:L31"/>
+    <mergeCell ref="M28:M31"/>
+    <mergeCell ref="N28:N31"/>
+    <mergeCell ref="O28:O31"/>
+    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="M15:M18"/>
+    <mergeCell ref="N15:N18"/>
+    <mergeCell ref="O15:O18"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="H9:H13"/>
+    <mergeCell ref="I9:I13"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="B9:B36"/>
+    <mergeCell ref="A9:A13"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="G19:I28 G32:I36">
@@ -3016,16 +3015,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="24" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -3037,16 +3036,16 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="27">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="37">
         <v>46113</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3058,16 +3057,16 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3079,11 +3078,11 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -3104,9 +3103,9 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="11">
         <v>0</v>
       </c>
@@ -3208,122 +3207,122 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="41">
+      <c r="A9" s="38">
         <v>1</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="L9" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28" t="s">
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
     </row>
     <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="8" t="s">
         <v>146</v>
       </c>
@@ -3358,103 +3357,103 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="41">
+      <c r="A15" s="38">
         <v>3</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="42" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="G15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K15" s="28" t="s">
+      <c r="K15" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="L15" s="28" t="s">
+      <c r="L15" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="34" t="s">
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="35"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="20"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="35"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="20"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="36"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="21"/>
     </row>
     <row r="19" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>4</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="19" t="s">
         <v>133</v>
       </c>
       <c r="D19" s="8" t="s">
@@ -3494,8 +3493,8 @@
       <c r="A20" s="7">
         <v>5</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="8" t="s">
         <v>150</v>
       </c>
@@ -3533,8 +3532,8 @@
       <c r="A21" s="7">
         <v>6</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="8" t="s">
         <v>151</v>
       </c>
@@ -3573,8 +3572,8 @@
         <f>SUM(A21+1)</f>
         <v>7</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="8" t="s">
         <v>152</v>
       </c>
@@ -3613,8 +3612,8 @@
         <f t="shared" ref="A23" si="0">SUM(A22+1)</f>
         <v>8</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="8" t="s">
         <v>153</v>
       </c>
@@ -3651,10 +3650,10 @@
         <f>SUM(A23+1)</f>
         <v>9</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="19" t="s">
         <v>134</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -3695,8 +3694,8 @@
         <f>SUM(A24+1)</f>
         <v>10</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="8" t="s">
         <v>170</v>
       </c>
@@ -3735,8 +3734,8 @@
         <f t="shared" ref="A26:A28" si="1">SUM(A25+1)</f>
         <v>11</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="8" t="s">
         <v>171</v>
       </c>
@@ -3773,8 +3772,8 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="8" t="s">
         <v>172</v>
       </c>
@@ -3811,8 +3810,8 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="8" t="s">
         <v>173</v>
       </c>
@@ -3848,18 +3847,17 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="J15:J18"/>
-    <mergeCell ref="K15:K18"/>
-    <mergeCell ref="L15:L18"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="L9:L13"/>
-    <mergeCell ref="M9:M13"/>
-    <mergeCell ref="N9:N13"/>
-    <mergeCell ref="O9:O13"/>
-    <mergeCell ref="N15:N18"/>
-    <mergeCell ref="O15:O18"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="J9:J13"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="A9:A13"/>
@@ -3876,17 +3874,18 @@
     <mergeCell ref="D15:D18"/>
     <mergeCell ref="E15:E18"/>
     <mergeCell ref="F15:F18"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="M15:M18"/>
+    <mergeCell ref="L9:L13"/>
+    <mergeCell ref="M9:M13"/>
+    <mergeCell ref="N9:N13"/>
+    <mergeCell ref="O9:O13"/>
+    <mergeCell ref="N15:N18"/>
+    <mergeCell ref="O15:O18"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="K15:K18"/>
+    <mergeCell ref="L15:L18"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="G19:I28">
@@ -3964,10 +3963,10 @@
   </sheetPr>
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3990,16 +3989,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="24" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -4011,16 +4010,16 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="27">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="37">
         <v>46113</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -4032,16 +4031,16 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -4053,11 +4052,11 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -4078,9 +4077,9 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="11">
         <v>0</v>
       </c>
@@ -4135,49 +4134,49 @@
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="44" t="s">
+      <c r="H8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="44" t="s">
+      <c r="I8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="44" t="s">
+      <c r="K8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="44" t="s">
+      <c r="L8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="44" t="s">
+      <c r="M8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="44" t="s">
+      <c r="N8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="44" t="s">
+      <c r="O8" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4185,14 +4184,14 @@
       <c r="A9" s="9">
         <v>1</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>187</v>
-      </c>
-      <c r="C9" s="43" t="s">
+      <c r="B9" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="40" t="s">
         <v>177</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>174</v>
@@ -4229,10 +4228,10 @@
         <f t="shared" ref="A10:A11" si="0">SUM(A9+1)</f>
         <v>2</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>175</v>
@@ -4253,10 +4252,10 @@
         <v>97</v>
       </c>
       <c r="K10" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>181</v>
       </c>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
@@ -4269,10 +4268,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>176</v>
@@ -4293,10 +4292,10 @@
         <v>97</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>

</xml_diff>